<commit_message>
QB Website updated 12/13
</commit_message>
<xml_diff>
--- a/Data/ChildCareSubsidyCC.xlsx
+++ b/Data/ChildCareSubsidyCC.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24617"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -62,7 +62,7 @@
     <t>RAPID Team</t>
   </si>
   <si>
-    <t>36</t>
+    <t>36, 40</t>
   </si>
   <si>
     <t>What percentage of families in your program use government subsidies to pay for child care?</t>
@@ -87,6 +87,38 @@
   </si>
   <si>
     <t xml:space="preserve">How does including government funding support your program? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: I am concerned about the staff recruitment crisis </t>
+  </si>
+  <si>
+    <t>● Strongly agree
+● Agree
+● Neither agree nor disagree
+● Disagree
+● Strongly disagree
+● N/A</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: I am concerned about retaining the employees I do have </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: I am concerned about how I am going to stay afloat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: I am concerned about how I am going to afford higher wages for my myself and employees </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: I am concerned about how I am going to afford benefits for my myself and employees </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please  rate your level of agreement with the following statement: Federal support would allow me to provide higher wages and benefits to myself my employees </t>
+  </si>
+  <si>
+    <t>Please  rate your level of agreement with the following statement: Federal support would allow me to stay afloat</t>
   </si>
 </sst>
 </file>
@@ -137,7 +169,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -173,11 +205,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -198,14 +239,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1369,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1"/>
@@ -1416,7 +1454,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="242.25" customHeight="1">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1472,53 +1510,95 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="102" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="153" customHeight="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="153" customHeight="1">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
+      <c r="A9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="153" customHeight="1">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
+      <c r="A10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="102" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
+      <c r="A11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="170.1" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
+      <c r="A12" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="102" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
+      <c r="A13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="76.5" customHeight="1">
       <c r="A14" s="7"/>

</xml_diff>